<commit_message>
Bigger font on chart
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="-20980" windowWidth="20240" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -972,11 +972,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2102357224"/>
-        <c:axId val="2102243208"/>
+        <c:axId val="2073035800"/>
+        <c:axId val="2076218216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2102357224"/>
+        <c:axId val="2073035800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,7 +985,17 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102243208"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2076218216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -993,7 +1003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2102243208"/>
+        <c:axId val="2076218216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -1010,7 +1020,17 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2102357224"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2073035800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1019,6 +1039,16 @@
       <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1399,7 +1429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -1952,6 +1982,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1966,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>